<commit_message>
Added the funcionality to set the GlobalConfig-Register and the MuxDelayRegister for each LTC2983 present on the card via reg2 and reg3 from the IP-Core changes for the driver still pending
</commit_message>
<xml_diff>
--- a/ip_cores/Temperature_Card_Interfrace_V1/Registermap_UZ_TempCard.xlsx
+++ b/ip_cores/Temperature_Card_Interfrace_V1/Registermap_UZ_TempCard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_Repos\Ultrazohm\ultrazohm_sw\ip_cores\Temperature_Card_Interfrace_V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04F1189-EE0E-447F-ADF4-F173D07155F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B90BEB3-1CAF-48B3-B321-EF9BFB1692EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20565" yWindow="2310" windowWidth="27150" windowHeight="15825" xr2:uid="{0C5271F0-7C67-4F7B-AE54-96CEBD1FEC7D}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0C5271F0-7C67-4F7B-AE54-96CEBD1FEC7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="97">
   <si>
     <t>Registermap UltraZohm Temperature Card</t>
   </si>
@@ -310,6 +310,21 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>GlobalConfig_Reg</t>
+  </si>
+  <si>
+    <t>MuxConfig_Reg</t>
+  </si>
+  <si>
+    <t>Channel_A</t>
+  </si>
+  <si>
+    <t>Channel_B</t>
+  </si>
+  <si>
+    <t>Channel_C</t>
   </si>
 </sst>
 </file>
@@ -360,13 +375,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF889AF-C6D6-402A-BECE-9F8C99140D0E}">
   <dimension ref="A1:AK135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,31 +712,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -729,7 +744,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -921,9 +936,42 @@
         <f t="shared" si="1"/>
         <v>A0000008</v>
       </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
       <c r="E10" t="s">
         <v>88</v>
       </c>
+      <c r="N10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -937,9 +985,42 @@
         <f t="shared" si="1"/>
         <v>A000000C</v>
       </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
       <c r="E11" t="s">
         <v>88</v>
       </c>
+      <c r="N11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -3292,8 +3373,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
     <mergeCell ref="A1:I2"/>
+    <mergeCell ref="AD11:AK11"/>
+    <mergeCell ref="V11:AC11"/>
+    <mergeCell ref="N11:U11"/>
+    <mergeCell ref="N10:U10"/>
+    <mergeCell ref="V10:AC10"/>
+    <mergeCell ref="AD10:AK10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>